<commit_message>
Manually merge to fix conflits
</commit_message>
<xml_diff>
--- a/tests/Stubs/SuccessInvoiceImportFile.xlsx
+++ b/tests/Stubs/SuccessInvoiceImportFile.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t xml:space="preserve">Client</t>
   </si>
@@ -87,21 +87,6 @@
   </si>
   <si>
     <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RKB910</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voluptatem vitae.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MNZ768</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Id et.</t>
   </si>
   <si>
     <t xml:space="preserve">sent</t>
@@ -111,15 +96,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="[$-409]General"/>
-    <numFmt numFmtId="165" formatCode="[$-409][$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="[H]:MM:SS"/>
     <numFmt numFmtId="167" formatCode="[$-409]@"/>
-    <numFmt numFmtId="168" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
-    <numFmt numFmtId="169" formatCode="[$-409]0.00%"/>
+    <numFmt numFmtId="168" formatCode="[$-409]0.00%"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -270,11 +254,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -593,7 +572,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -650,23 +629,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -790,22 +765,19 @@
   <dimension ref="A2:J40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="A9:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.75"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="4.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="4.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.59"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -865,7 +837,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>970717226</v>
+        <v>438044217</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="7" t="s">
@@ -875,7 +847,7 @@
         <v>10</v>
       </c>
       <c r="G5" s="4" t="n">
-        <v>265631438</v>
+        <v>966859957</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="5" t="s">
@@ -940,173 +912,147 @@
       <c r="J8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="n">
-        <v>3</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="14" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="E9" s="14" t="n">
-        <v>37.5</v>
-      </c>
-      <c r="F9" s="15" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>24</v>
-      </c>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="13"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="n">
-        <v>10</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="14" t="n">
-        <v>28.94</v>
-      </c>
-      <c r="E10" s="14" t="n">
-        <v>38.5</v>
-      </c>
-      <c r="F10" s="15" t="n">
-        <v>0.324</v>
-      </c>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
       <c r="J10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="17"/>
-      <c r="F11" s="18"/>
+      <c r="D11" s="16"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="17"/>
-      <c r="F12" s="18"/>
+      <c r="D12" s="16"/>
+      <c r="F12" s="17"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="17"/>
-      <c r="F13" s="18"/>
+      <c r="D13" s="16"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="17"/>
-      <c r="F14" s="18"/>
+      <c r="D14" s="16"/>
+      <c r="F14" s="17"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="17"/>
-      <c r="F15" s="18"/>
+      <c r="D15" s="16"/>
+      <c r="F15" s="17"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="17"/>
-      <c r="F16" s="18"/>
+      <c r="D16" s="16"/>
+      <c r="F16" s="17"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="17"/>
-      <c r="F17" s="18"/>
+      <c r="D17" s="16"/>
+      <c r="F17" s="17"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="17"/>
-      <c r="F18" s="18"/>
+      <c r="D18" s="16"/>
+      <c r="F18" s="17"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="17"/>
-      <c r="F19" s="18"/>
+      <c r="D19" s="16"/>
+      <c r="F19" s="17"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="17"/>
-      <c r="F20" s="18"/>
+      <c r="D20" s="16"/>
+      <c r="F20" s="17"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="17"/>
-      <c r="F21" s="18"/>
+      <c r="D21" s="16"/>
+      <c r="F21" s="17"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="17"/>
-      <c r="F22" s="18"/>
+      <c r="D22" s="16"/>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="17"/>
-      <c r="F23" s="18"/>
+      <c r="D23" s="16"/>
+      <c r="F23" s="17"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="17"/>
-      <c r="F24" s="18"/>
+      <c r="D24" s="16"/>
+      <c r="F24" s="17"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="17"/>
-      <c r="F25" s="18"/>
+      <c r="D25" s="16"/>
+      <c r="F25" s="17"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="17"/>
-      <c r="F26" s="18"/>
+      <c r="D26" s="16"/>
+      <c r="F26" s="17"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="17"/>
-      <c r="F27" s="18"/>
+      <c r="D27" s="16"/>
+      <c r="F27" s="17"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="17"/>
-      <c r="F28" s="18"/>
+      <c r="D28" s="16"/>
+      <c r="F28" s="17"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="17"/>
-      <c r="F29" s="18"/>
+      <c r="D29" s="16"/>
+      <c r="F29" s="17"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="17"/>
-      <c r="F30" s="18"/>
+      <c r="D30" s="16"/>
+      <c r="F30" s="17"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="17"/>
-      <c r="F31" s="18"/>
+      <c r="D31" s="16"/>
+      <c r="F31" s="17"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="17"/>
-      <c r="F32" s="18"/>
+      <c r="D32" s="16"/>
+      <c r="F32" s="17"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="17"/>
-      <c r="F33" s="18"/>
+      <c r="D33" s="16"/>
+      <c r="F33" s="17"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="17"/>
-      <c r="F34" s="18"/>
+      <c r="D34" s="16"/>
+      <c r="F34" s="17"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="17"/>
-      <c r="F35" s="18"/>
+      <c r="D35" s="16"/>
+      <c r="F35" s="17"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="17"/>
-      <c r="F36" s="18"/>
+      <c r="D36" s="16"/>
+      <c r="F36" s="17"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="17"/>
-      <c r="F37" s="18"/>
+      <c r="D37" s="16"/>
+      <c r="F37" s="17"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="17"/>
-      <c r="F38" s="18"/>
+      <c r="D38" s="16"/>
+      <c r="F38" s="17"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D39" s="17"/>
-      <c r="F39" s="18"/>
+      <c r="D39" s="16"/>
+      <c r="F39" s="17"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F40" s="18"/>
+      <c r="F40" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1133,26 +1079,26 @@
   <dimension ref="A2:J97"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="A9:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="13.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="9" width="10.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="9" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="9" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="9.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="5.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="16.81"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="4" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="4" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="19"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
@@ -1205,7 +1151,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>970717226</v>
+        <v>438044217</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>9</v>
@@ -1214,7 +1160,7 @@
         <v>10</v>
       </c>
       <c r="G5" s="4" t="n">
-        <v>265631438</v>
+        <v>966859957</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>11</v>
@@ -1228,53 +1174,38 @@
         <v>13</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="20"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="20"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="n">
-        <v>3</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="14" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="E9" s="14" t="n">
-        <f aca="false">D9*A9</f>
-        <v>37.5</v>
-      </c>
-      <c r="F9" s="15" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>24</v>
-      </c>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="13"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
     </row>

</xml_diff>